<commit_message>
update data + server now online in local network
</commit_message>
<xml_diff>
--- a/TeslaNumbers.xlsx
+++ b/TeslaNumbers.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="34">
   <si>
     <t>quarter</t>
   </si>
@@ -22,25 +22,28 @@
     <t>revenue</t>
   </si>
   <si>
-    <t>carRevenue</t>
-  </si>
-  <si>
-    <t>carCostOfRevenue</t>
-  </si>
-  <si>
-    <t>deliveriesModel3Y</t>
-  </si>
-  <si>
-    <t>deliveriesOtherModels</t>
-  </si>
-  <si>
-    <t>productionModel3Y</t>
-  </si>
-  <si>
-    <t>productionOtherModels</t>
-  </si>
-  <si>
-    <t>carNumCars</t>
+    <t>automotiveRevenue</t>
+  </si>
+  <si>
+    <t>automotiveCostOfRevenue</t>
+  </si>
+  <si>
+    <t>deliveredModel3Y</t>
+  </si>
+  <si>
+    <t>deliveredOtherModels</t>
+  </si>
+  <si>
+    <t>producedModel3Y</t>
+  </si>
+  <si>
+    <t>producedOtherModels</t>
+  </si>
+  <si>
+    <t>producedCars</t>
+  </si>
+  <si>
+    <t>deliveredCars</t>
   </si>
   <si>
     <t>energyRevenue</t>
@@ -1368,14 +1371,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="13" width="16.3516" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="14" width="16.3516" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="32.25" customHeight="1">
@@ -1418,10 +1421,13 @@
       <c r="M1" t="s" s="2">
         <v>12</v>
       </c>
+      <c r="N1" t="s" s="2">
+        <v>13</v>
+      </c>
     </row>
     <row r="2" ht="20.25" customHeight="1">
       <c r="A2" t="s" s="3">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B2" s="4">
         <f>0.566*10^9</f>
@@ -1450,22 +1456,26 @@
         <v>14163</v>
       </c>
       <c r="J2" s="5">
+        <f>H2+I2</f>
+        <v>77138</v>
+      </c>
+      <c r="K2" s="5">
         <f>F2+G2</f>
         <v>63019</v>
       </c>
-      <c r="K2" s="5">
+      <c r="L2" s="5">
         <v>324000000</v>
       </c>
-      <c r="L2" s="5">
+      <c r="M2" s="5">
         <v>316000000</v>
       </c>
-      <c r="M2" s="5">
+      <c r="N2" s="5">
         <v>229000000000</v>
       </c>
     </row>
     <row r="3" ht="20.05" customHeight="1">
       <c r="A3" t="s" s="6">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B3" s="7">
         <f>0.921*10^9</f>
@@ -1494,22 +1504,26 @@
         <v>14517</v>
       </c>
       <c r="J3" s="8">
+        <f>H3+I3</f>
+        <v>87048</v>
+      </c>
+      <c r="K3" s="8">
         <f>F3+G3</f>
         <v>95356</v>
       </c>
-      <c r="K3" s="8">
+      <c r="L3" s="8">
         <v>369000000</v>
       </c>
-      <c r="L3" s="8">
+      <c r="M3" s="8">
         <v>326000000</v>
       </c>
-      <c r="M3" s="8">
+      <c r="N3" s="8">
         <v>415000000000</v>
       </c>
     </row>
     <row r="4" ht="20.05" customHeight="1">
       <c r="A4" t="s" s="6">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B4" s="7">
         <f>1.191*10^9</f>
@@ -1538,22 +1552,26 @@
         <v>16318</v>
       </c>
       <c r="J4" s="8">
+        <f>H4+I4</f>
+        <v>96155</v>
+      </c>
+      <c r="K4" s="8">
         <f>F4+G4</f>
         <v>97186</v>
       </c>
-      <c r="K4" s="8">
+      <c r="L4" s="8">
         <v>402000000</v>
       </c>
-      <c r="L4" s="8">
+      <c r="M4" s="8">
         <v>314000000</v>
       </c>
-      <c r="M4" s="8">
+      <c r="N4" s="8">
         <v>477000000000</v>
       </c>
     </row>
     <row r="5" ht="20.05" customHeight="1">
       <c r="A5" t="s" s="6">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B5" s="7">
         <f>1.391*10^9</f>
@@ -1582,22 +1600,26 @@
         <v>17933</v>
       </c>
       <c r="J5" s="8">
+        <f>H5+I5</f>
+        <v>104891</v>
+      </c>
+      <c r="K5" s="8">
         <f>F5+G5</f>
         <v>112095</v>
       </c>
-      <c r="K5" s="8">
+      <c r="L5" s="8">
         <v>436000000</v>
       </c>
-      <c r="L5" s="8">
+      <c r="M5" s="8">
         <v>385000000</v>
       </c>
-      <c r="M5" s="8">
+      <c r="N5" s="8">
         <v>530000000000</v>
       </c>
     </row>
     <row r="6" ht="20.05" customHeight="1">
       <c r="A6" t="s" s="6">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B6" s="7">
         <f>1.234*10^9</f>
@@ -1626,22 +1648,26 @@
         <v>15390</v>
       </c>
       <c r="J6" s="8">
+        <f>H6+I6</f>
+        <v>102672</v>
+      </c>
+      <c r="K6" s="8">
         <f>F6+G6</f>
         <v>88496</v>
       </c>
-      <c r="K6" s="8">
+      <c r="L6" s="8">
         <v>293000000</v>
       </c>
-      <c r="L6" s="8">
+      <c r="M6" s="8">
         <v>282000000</v>
       </c>
-      <c r="M6" s="8">
+      <c r="N6" s="8">
         <v>260000000000</v>
       </c>
     </row>
     <row r="7" ht="20.05" customHeight="1">
       <c r="A7" t="s" s="6">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B7" s="7">
         <f>1.267*10^9</f>
@@ -1670,22 +1696,26 @@
         <v>6326</v>
       </c>
       <c r="J7" s="8">
+        <f>H7+I7</f>
+        <v>82272</v>
+      </c>
+      <c r="K7" s="8">
         <f>F7+G7</f>
         <v>90891</v>
       </c>
-      <c r="K7" s="8">
+      <c r="L7" s="8">
         <v>370000000</v>
       </c>
-      <c r="L7" s="8">
+      <c r="M7" s="8">
         <v>349000000</v>
       </c>
-      <c r="M7" s="8">
+      <c r="N7" s="8">
         <v>419000000000</v>
       </c>
     </row>
     <row r="8" ht="20.05" customHeight="1">
       <c r="A8" t="s" s="6">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B8" s="7">
         <f>2.063*10^9</f>
@@ -1714,22 +1744,26 @@
         <v>16992</v>
       </c>
       <c r="J8" s="8">
+        <f>H8+I8</f>
+        <v>145036</v>
+      </c>
+      <c r="K8" s="8">
         <f>F8+G8</f>
         <v>139593</v>
       </c>
-      <c r="K8" s="8">
+      <c r="L8" s="8">
         <v>579000000</v>
       </c>
-      <c r="L8" s="8">
+      <c r="M8" s="8">
         <v>558000000</v>
       </c>
-      <c r="M8" s="8">
+      <c r="N8" s="8">
         <v>759000000000</v>
       </c>
     </row>
     <row r="9" ht="20.05" customHeight="1">
       <c r="A9" t="s" s="6">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B9" s="7">
         <f>2.066*10^9</f>
@@ -1758,22 +1792,26 @@
         <v>16097</v>
       </c>
       <c r="J9" s="8">
+        <f>H9+I9</f>
+        <v>179757</v>
+      </c>
+      <c r="K9" s="8">
         <f>F9+G9</f>
         <v>180667</v>
       </c>
-      <c r="K9" s="8">
+      <c r="L9" s="8">
         <v>752000000</v>
       </c>
-      <c r="L9" s="8">
+      <c r="M9" s="8">
         <v>787000000</v>
       </c>
-      <c r="M9" s="8">
+      <c r="N9" s="8">
         <v>1584000000000</v>
       </c>
     </row>
     <row r="10" ht="20.05" customHeight="1">
       <c r="A10" t="s" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B10" s="7">
         <f>2.215*10^9</f>
@@ -1802,22 +1840,26 @@
         <v>0</v>
       </c>
       <c r="J10" s="8">
+        <f>H10+I10</f>
+        <v>180338</v>
+      </c>
+      <c r="K10" s="8">
         <f>F10+G10</f>
         <v>184877</v>
       </c>
-      <c r="K10" s="8">
+      <c r="L10" s="8">
         <v>494000000</v>
       </c>
-      <c r="L10" s="8">
+      <c r="M10" s="8">
         <v>595000000</v>
       </c>
-      <c r="M10" s="8">
+      <c r="N10" s="8">
         <v>445000000000</v>
       </c>
     </row>
     <row r="11" ht="20.05" customHeight="1">
       <c r="A11" t="s" s="6">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B11" s="7">
         <f>2.884*10^9</f>
@@ -1846,22 +1888,26 @@
         <v>2340</v>
       </c>
       <c r="J11" s="8">
+        <f>H11+I11</f>
+        <v>206421</v>
+      </c>
+      <c r="K11" s="8">
         <f>F11+G11</f>
         <v>201304</v>
       </c>
-      <c r="K11" s="8">
+      <c r="L11" s="8">
         <v>801000000</v>
       </c>
-      <c r="L11" s="8">
+      <c r="M11" s="8">
         <v>781000000</v>
       </c>
-      <c r="M11" s="8">
+      <c r="N11" s="8">
         <v>1274000000000</v>
       </c>
     </row>
     <row r="12" ht="20.05" customHeight="1">
       <c r="A12" t="s" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B12" s="7">
         <f>3.66*10^9</f>
@@ -1890,22 +1936,26 @@
         <v>8941</v>
       </c>
       <c r="J12" s="8">
+        <f>H12+I12</f>
+        <v>237823</v>
+      </c>
+      <c r="K12" s="8">
         <f>F12+G12</f>
         <v>241391</v>
       </c>
-      <c r="K12" s="8">
+      <c r="L12" s="8">
         <v>806000000</v>
       </c>
-      <c r="L12" s="8">
+      <c r="M12" s="8">
         <v>803000000</v>
       </c>
-      <c r="M12" s="8">
+      <c r="N12" s="8">
         <v>1295000000000</v>
       </c>
     </row>
     <row r="13" ht="20.05" customHeight="1">
       <c r="A13" t="s" s="6">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B13" s="7">
         <f>4.847*10^9</f>
@@ -1934,22 +1984,26 @@
         <v>13109</v>
       </c>
       <c r="J13" s="8">
+        <f>H13+I13</f>
+        <v>305840</v>
+      </c>
+      <c r="K13" s="8">
         <f>F13+G13</f>
         <v>308650</v>
       </c>
-      <c r="K13" s="8">
+      <c r="L13" s="8">
         <v>688000000</v>
       </c>
-      <c r="L13" s="8">
+      <c r="M13" s="8">
         <v>739000000</v>
       </c>
-      <c r="M13" s="8">
+      <c r="N13" s="8">
         <v>978000000000</v>
       </c>
     </row>
     <row r="14" ht="20.05" customHeight="1">
       <c r="A14" t="s" s="6">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B14" s="7">
         <f>5.46*10^9</f>
@@ -1978,22 +2032,26 @@
         <v>14218</v>
       </c>
       <c r="J14" s="8">
+        <f>H14+I14</f>
+        <v>305407</v>
+      </c>
+      <c r="K14" s="8">
         <f>F14+G14</f>
         <v>310048</v>
       </c>
-      <c r="K14" s="8">
+      <c r="L14" s="8">
         <v>616000000</v>
       </c>
-      <c r="L14" s="8">
+      <c r="M14" s="8">
         <v>688000000</v>
       </c>
-      <c r="M14" s="8">
+      <c r="N14" s="8">
         <v>846000000000</v>
       </c>
     </row>
     <row r="15" ht="20.05" customHeight="1">
       <c r="A15" t="s" s="6">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B15" s="7">
         <f>4.234*10^9</f>
@@ -2022,22 +2080,26 @@
         <v>16411</v>
       </c>
       <c r="J15" s="8">
+        <f>H15+I15</f>
+        <v>258580</v>
+      </c>
+      <c r="K15" s="8">
         <f>F15+G15</f>
         <v>254695</v>
       </c>
-      <c r="K15" s="8">
+      <c r="L15" s="8">
         <v>866000000</v>
       </c>
-      <c r="L15" s="8">
+      <c r="M15" s="8">
         <v>769000000</v>
       </c>
-      <c r="M15" s="8">
+      <c r="N15" s="8">
         <v>1133000000000</v>
       </c>
     </row>
     <row r="16" ht="20.05" customHeight="1">
       <c r="A16" t="s" s="6">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B16" s="7">
         <f>5.382*10^9</f>
@@ -2066,22 +2128,26 @@
         <v>19935</v>
       </c>
       <c r="J16" s="8">
+        <f>H16+I16</f>
+        <v>365923</v>
+      </c>
+      <c r="K16" s="8">
         <f>F16+G16</f>
         <v>343830</v>
       </c>
-      <c r="K16" s="8">
+      <c r="L16" s="8">
         <v>1117000000</v>
       </c>
-      <c r="L16" s="8">
+      <c r="M16" s="8">
         <v>1101300000</v>
       </c>
-      <c r="M16" s="8">
+      <c r="N16" s="8">
         <v>2100000000000</v>
       </c>
     </row>
     <row r="17" ht="20.05" customHeight="1">
       <c r="A17" t="s" s="6">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B17" s="7">
         <f>5.777*10^9</f>
@@ -2110,22 +2176,26 @@
         <v>20613</v>
       </c>
       <c r="J17" s="8">
+        <f>H17+I17</f>
+        <v>439701</v>
+      </c>
+      <c r="K17" s="8">
         <f>F17+G17</f>
         <v>405278</v>
       </c>
-      <c r="K17" s="8">
+      <c r="L17" s="8">
         <v>1310000000</v>
       </c>
-      <c r="L17" s="8">
+      <c r="M17" s="8">
         <v>1151000000</v>
       </c>
-      <c r="M17" s="8">
+      <c r="N17" s="8">
         <v>2462000000000</v>
       </c>
     </row>
     <row r="18" ht="20.05" customHeight="1">
       <c r="A18" t="s" s="6">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B18" s="7">
         <f>4.511*10^9</f>
@@ -2154,22 +2224,26 @@
         <v>19437</v>
       </c>
       <c r="J18" s="8">
+        <f>H18+I18</f>
+        <v>440808</v>
+      </c>
+      <c r="K18" s="8">
         <f>F18+G18</f>
         <v>422875</v>
       </c>
-      <c r="K18" s="8">
+      <c r="L18" s="8">
         <v>1529000000</v>
       </c>
-      <c r="L18" s="8">
+      <c r="M18" s="8">
         <v>1361000000</v>
       </c>
-      <c r="M18" s="8">
+      <c r="N18" s="8">
         <v>3889000000000</v>
       </c>
     </row>
     <row r="19" ht="20.05" customHeight="1">
       <c r="A19" t="s" s="6">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B19" s="7">
         <f>4.533*10^9</f>
@@ -2198,22 +2272,26 @@
         <v>19489</v>
       </c>
       <c r="J19" s="8">
+        <f>H19+I19</f>
+        <v>479700</v>
+      </c>
+      <c r="K19" s="8">
         <f>F19+G19</f>
         <v>466140</v>
       </c>
-      <c r="K19" s="8">
+      <c r="L19" s="8">
         <v>1509000000</v>
       </c>
-      <c r="L19" s="8">
+      <c r="M19" s="8">
         <v>1231000000</v>
       </c>
-      <c r="M19" s="8">
+      <c r="N19" s="8">
         <v>3653000000000</v>
       </c>
     </row>
     <row r="20" ht="20.05" customHeight="1">
       <c r="A20" t="s" s="6">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B20" s="7">
         <f>4.178*10^9</f>
@@ -2242,22 +2320,26 @@
         <v>13688</v>
       </c>
       <c r="J20" s="8">
+        <f>H20+I20</f>
+        <v>430488</v>
+      </c>
+      <c r="K20" s="8">
         <f>F20+G20</f>
         <v>435059</v>
       </c>
-      <c r="K20" s="8">
+      <c r="L20" s="8">
         <v>1559000000</v>
       </c>
-      <c r="L20" s="8">
+      <c r="M20" s="8">
         <v>1178000000</v>
       </c>
-      <c r="M20" s="8">
+      <c r="N20" s="8">
         <v>3980000000000</v>
       </c>
     </row>
     <row r="21" ht="20.05" customHeight="1">
       <c r="A21" t="s" s="6">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B21" s="7">
         <v>4438000000</v>
@@ -2284,15 +2366,19 @@
         <v>18212</v>
       </c>
       <c r="J21" s="8">
+        <f>H21+I21</f>
+        <v>494989</v>
+      </c>
+      <c r="K21" s="8">
         <v>484507</v>
       </c>
-      <c r="K21" s="8">
+      <c r="L21" s="8">
         <v>1438000000</v>
       </c>
-      <c r="L21" s="8">
+      <c r="M21" s="8">
         <v>1124000000</v>
       </c>
-      <c r="M21" s="8">
+      <c r="N21" s="8">
         <v>3202000000000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update TeslaNumbers with new data
</commit_message>
<xml_diff>
--- a/TeslaNumbers.xlsx
+++ b/TeslaNumbers.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="37">
   <si>
     <t>quarter</t>
   </si>
@@ -53,6 +53,15 @@
   </si>
   <si>
     <t>energyStorage</t>
+  </si>
+  <si>
+    <t>solarDeployed</t>
+  </si>
+  <si>
+    <t>superchargerStationsAccumulated</t>
+  </si>
+  <si>
+    <t>superchargerConnectorsAccumulated</t>
   </si>
   <si>
     <t>Q1 2019</t>
@@ -1371,14 +1380,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:N21"/>
+  <dimension ref="A1:Q21"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="14" width="16.3516" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="17" width="16.3516" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="32.25" customHeight="1">
@@ -1424,10 +1433,19 @@
       <c r="N1" t="s" s="2">
         <v>13</v>
       </c>
+      <c r="O1" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s" s="2">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s" s="2">
+        <v>16</v>
+      </c>
     </row>
     <row r="2" ht="20.25" customHeight="1">
       <c r="A2" t="s" s="3">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B2" s="4">
         <f>0.566*10^9</f>
@@ -1472,10 +1490,19 @@
       <c r="N2" s="5">
         <v>229000000000</v>
       </c>
+      <c r="O2" s="5">
+        <v>47</v>
+      </c>
+      <c r="P2" s="5">
+        <v>1490</v>
+      </c>
+      <c r="Q2" s="5">
+        <v>12767</v>
+      </c>
     </row>
     <row r="3" ht="20.05" customHeight="1">
       <c r="A3" t="s" s="6">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B3" s="7">
         <f>0.921*10^9</f>
@@ -1520,10 +1547,19 @@
       <c r="N3" s="8">
         <v>415000000000</v>
       </c>
+      <c r="O3" s="8">
+        <v>29</v>
+      </c>
+      <c r="P3" s="8">
+        <v>1587</v>
+      </c>
+      <c r="Q3" s="8">
+        <v>13881</v>
+      </c>
     </row>
     <row r="4" ht="20.05" customHeight="1">
       <c r="A4" t="s" s="6">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B4" s="7">
         <f>1.191*10^9</f>
@@ -1568,10 +1604,19 @@
       <c r="N4" s="8">
         <v>477000000000</v>
       </c>
+      <c r="O4" s="8">
+        <v>43</v>
+      </c>
+      <c r="P4" s="8">
+        <v>1653</v>
+      </c>
+      <c r="Q4" s="8">
+        <v>14658</v>
+      </c>
     </row>
     <row r="5" ht="20.05" customHeight="1">
       <c r="A5" t="s" s="6">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B5" s="7">
         <f>1.391*10^9</f>
@@ -1616,10 +1661,19 @@
       <c r="N5" s="8">
         <v>530000000000</v>
       </c>
+      <c r="O5" s="8">
+        <v>54</v>
+      </c>
+      <c r="P5" s="8">
+        <v>1821</v>
+      </c>
+      <c r="Q5" s="8">
+        <v>16104</v>
+      </c>
     </row>
     <row r="6" ht="20.05" customHeight="1">
       <c r="A6" t="s" s="6">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B6" s="7">
         <f>1.234*10^9</f>
@@ -1664,10 +1718,19 @@
       <c r="N6" s="8">
         <v>260000000000</v>
       </c>
+      <c r="O6" s="8">
+        <v>35</v>
+      </c>
+      <c r="P6" s="8">
+        <v>1917</v>
+      </c>
+      <c r="Q6" s="8">
+        <v>17007</v>
+      </c>
     </row>
     <row r="7" ht="20.05" customHeight="1">
       <c r="A7" t="s" s="6">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B7" s="7">
         <f>1.267*10^9</f>
@@ -1712,10 +1775,19 @@
       <c r="N7" s="8">
         <v>419000000000</v>
       </c>
+      <c r="O7" s="8">
+        <v>27</v>
+      </c>
+      <c r="P7" s="8">
+        <v>2035</v>
+      </c>
+      <c r="Q7" s="8">
+        <v>18100</v>
+      </c>
     </row>
     <row r="8" ht="20.05" customHeight="1">
       <c r="A8" t="s" s="6">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B8" s="7">
         <f>2.063*10^9</f>
@@ -1760,10 +1832,19 @@
       <c r="N8" s="8">
         <v>759000000000</v>
       </c>
+      <c r="O8" s="8">
+        <v>57</v>
+      </c>
+      <c r="P8" s="8">
+        <v>2181</v>
+      </c>
+      <c r="Q8" s="8">
+        <v>19437</v>
+      </c>
     </row>
     <row r="9" ht="20.05" customHeight="1">
       <c r="A9" t="s" s="6">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B9" s="7">
         <f>2.066*10^9</f>
@@ -1808,10 +1889,19 @@
       <c r="N9" s="8">
         <v>1584000000000</v>
       </c>
+      <c r="O9" s="8">
+        <v>86</v>
+      </c>
+      <c r="P9" s="8">
+        <v>2564</v>
+      </c>
+      <c r="Q9" s="8">
+        <v>23277</v>
+      </c>
     </row>
     <row r="10" ht="20.05" customHeight="1">
       <c r="A10" t="s" s="6">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B10" s="7">
         <f>2.215*10^9</f>
@@ -1856,10 +1946,19 @@
       <c r="N10" s="8">
         <v>445000000000</v>
       </c>
+      <c r="O10" s="8">
+        <v>92</v>
+      </c>
+      <c r="P10" s="8">
+        <v>2699</v>
+      </c>
+      <c r="Q10" s="8">
+        <v>24515</v>
+      </c>
     </row>
     <row r="11" ht="20.05" customHeight="1">
       <c r="A11" t="s" s="6">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B11" s="7">
         <f>2.884*10^9</f>
@@ -1904,10 +2003,19 @@
       <c r="N11" s="8">
         <v>1274000000000</v>
       </c>
+      <c r="O11" s="8">
+        <v>85</v>
+      </c>
+      <c r="P11" s="8">
+        <v>2966</v>
+      </c>
+      <c r="Q11" s="8">
+        <v>26900</v>
+      </c>
     </row>
     <row r="12" ht="20.05" customHeight="1">
       <c r="A12" t="s" s="6">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B12" s="7">
         <f>3.66*10^9</f>
@@ -1952,10 +2060,19 @@
       <c r="N12" s="8">
         <v>1295000000000</v>
       </c>
+      <c r="O12" s="8">
+        <v>83</v>
+      </c>
+      <c r="P12" s="8">
+        <v>3254</v>
+      </c>
+      <c r="Q12" s="8">
+        <v>29281</v>
+      </c>
     </row>
     <row r="13" ht="20.05" customHeight="1">
       <c r="A13" t="s" s="6">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B13" s="7">
         <f>4.847*10^9</f>
@@ -2000,10 +2117,19 @@
       <c r="N13" s="8">
         <v>978000000000</v>
       </c>
+      <c r="O13" s="8">
+        <v>85</v>
+      </c>
+      <c r="P13" s="8">
+        <v>3476</v>
+      </c>
+      <c r="Q13" s="8">
+        <v>31498</v>
+      </c>
     </row>
     <row r="14" ht="20.05" customHeight="1">
       <c r="A14" t="s" s="6">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B14" s="7">
         <f>5.46*10^9</f>
@@ -2048,10 +2174,19 @@
       <c r="N14" s="8">
         <v>846000000000</v>
       </c>
+      <c r="O14" s="8">
+        <v>48</v>
+      </c>
+      <c r="P14" s="8">
+        <v>3724</v>
+      </c>
+      <c r="Q14" s="8">
+        <v>33657</v>
+      </c>
     </row>
     <row r="15" ht="20.05" customHeight="1">
       <c r="A15" t="s" s="6">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B15" s="7">
         <f>4.234*10^9</f>
@@ -2096,10 +2231,19 @@
       <c r="N15" s="8">
         <v>1133000000000</v>
       </c>
+      <c r="O15" s="8">
+        <v>106</v>
+      </c>
+      <c r="P15" s="8">
+        <v>3971</v>
+      </c>
+      <c r="Q15" s="8">
+        <v>36165</v>
+      </c>
     </row>
     <row r="16" ht="20.05" customHeight="1">
       <c r="A16" t="s" s="6">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B16" s="7">
         <f>5.382*10^9</f>
@@ -2144,10 +2288,19 @@
       <c r="N16" s="8">
         <v>2100000000000</v>
       </c>
+      <c r="O16" s="8">
+        <v>94</v>
+      </c>
+      <c r="P16" s="8">
+        <v>4283</v>
+      </c>
+      <c r="Q16" s="8">
+        <v>38883</v>
+      </c>
     </row>
     <row r="17" ht="20.05" customHeight="1">
       <c r="A17" t="s" s="6">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B17" s="7">
         <f>5.777*10^9</f>
@@ -2192,10 +2345,19 @@
       <c r="N17" s="8">
         <v>2462000000000</v>
       </c>
+      <c r="O17" s="8">
+        <v>100</v>
+      </c>
+      <c r="P17" s="8">
+        <v>4678</v>
+      </c>
+      <c r="Q17" s="8">
+        <v>42419</v>
+      </c>
     </row>
     <row r="18" ht="20.05" customHeight="1">
       <c r="A18" t="s" s="6">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B18" s="7">
         <f>4.511*10^9</f>
@@ -2240,10 +2402,19 @@
       <c r="N18" s="8">
         <v>3889000000000</v>
       </c>
+      <c r="O18" s="8">
+        <v>67</v>
+      </c>
+      <c r="P18" s="8">
+        <v>4947</v>
+      </c>
+      <c r="Q18" s="8">
+        <v>45169</v>
+      </c>
     </row>
     <row r="19" ht="20.05" customHeight="1">
       <c r="A19" t="s" s="6">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B19" s="7">
         <f>4.533*10^9</f>
@@ -2288,10 +2459,19 @@
       <c r="N19" s="8">
         <v>3653000000000</v>
       </c>
+      <c r="O19" s="8">
+        <v>66</v>
+      </c>
+      <c r="P19" s="8">
+        <v>5265</v>
+      </c>
+      <c r="Q19" s="8">
+        <v>48082</v>
+      </c>
     </row>
     <row r="20" ht="20.05" customHeight="1">
       <c r="A20" t="s" s="6">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B20" s="7">
         <f>4.178*10^9</f>
@@ -2336,10 +2516,19 @@
       <c r="N20" s="8">
         <v>3980000000000</v>
       </c>
+      <c r="O20" s="8">
+        <v>49</v>
+      </c>
+      <c r="P20" s="8">
+        <v>5595</v>
+      </c>
+      <c r="Q20" s="8">
+        <v>51105</v>
+      </c>
     </row>
     <row r="21" ht="20.05" customHeight="1">
       <c r="A21" t="s" s="6">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B21" s="7">
         <v>4438000000</v>
@@ -2380,6 +2569,15 @@
       </c>
       <c r="N21" s="8">
         <v>3202000000000</v>
+      </c>
+      <c r="O21" s="8">
+        <v>41</v>
+      </c>
+      <c r="P21" s="8">
+        <v>5952</v>
+      </c>
+      <c r="Q21" s="8">
+        <v>54892</v>
       </c>
     </row>
   </sheetData>

</xml_diff>